<commit_message>
add dev part to scrum
</commit_message>
<xml_diff>
--- a/Docs/Scrum.xlsx
+++ b/Docs/Scrum.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
   <si>
     <t>Status</t>
   </si>
@@ -120,15 +120,9 @@
     <t xml:space="preserve">The file can be send by mail, Bluetooth…. </t>
   </si>
   <si>
-    <t>Vayan lama</t>
-  </si>
-  <si>
     <t>Ongoing</t>
   </si>
   <si>
-    <t>dev</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Buffer Record</t>
   </si>
   <si>
@@ -178,6 +172,24 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>Yann Vaillant</t>
+  </si>
+  <si>
+    <t>Maitre Robin</t>
+  </si>
+  <si>
+    <t>Yuyi</t>
+  </si>
+  <si>
+    <t>FENG Changhong</t>
+  </si>
+  <si>
+    <t>XIAO KAI</t>
+  </si>
+  <si>
+    <t>SUN Hao</t>
   </si>
 </sst>
 </file>
@@ -347,25 +359,25 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -392,57 +404,10 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.59999389629810485"/>
-          <bgColor theme="4" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="0"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -767,6 +732,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -779,10 +751,50 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -795,39 +807,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:K10"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Title/User Story" dataDxfId="22"/>
-    <tableColumn id="2" name="Description/Activity" dataDxfId="21"/>
-    <tableColumn id="3" name="Prio_x000a_(1 = high)" dataDxfId="20"/>
-    <tableColumn id="4" name="Status" dataDxfId="19"/>
-    <tableColumn id="5" name="Start Date" dataDxfId="18"/>
+    <tableColumn id="1" name="Title/User Story" dataDxfId="20"/>
+    <tableColumn id="2" name="Description/Activity" dataDxfId="19"/>
+    <tableColumn id="3" name="Prio_x000a_(1 = high)" dataDxfId="18"/>
+    <tableColumn id="4" name="Status" dataDxfId="17"/>
+    <tableColumn id="5" name="Start Date" dataDxfId="16"/>
     <tableColumn id="6" name="Est Time (weeks or  days)"/>
-    <tableColumn id="7" name="Estimated Time_x000a_S/M/L (1d/2d/3d)" dataDxfId="17"/>
+    <tableColumn id="7" name="Estimated Time_x000a_S/M/L (1d/2d/3d)" dataDxfId="15"/>
     <tableColumn id="8" name="Days"/>
-    <tableColumn id="9" name="Actual Time" dataDxfId="16"/>
-    <tableColumn id="10" name="Planned Sprint" dataDxfId="15"/>
-    <tableColumn id="11" name="Comment" dataDxfId="14"/>
+    <tableColumn id="9" name="Actual Time" dataDxfId="14"/>
+    <tableColumn id="10" name="Planned Sprint" dataDxfId="13"/>
+    <tableColumn id="11" name="Comment" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J10"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Title/User Story" dataDxfId="10"/>
-    <tableColumn id="2" name="Description/Activity" dataDxfId="9"/>
-    <tableColumn id="3" name="Priority_x000a_(1 = high)" dataDxfId="8"/>
-    <tableColumn id="4" name="Estimated Time" dataDxfId="7"/>
-    <tableColumn id="5" name="Started/used" dataDxfId="6"/>
-    <tableColumn id="6" name="Completion used" dataDxfId="5"/>
-    <tableColumn id="7" name="Developer" dataDxfId="4"/>
-    <tableColumn id="8" name="Status" dataDxfId="3"/>
-    <tableColumn id="9" name="Week" dataDxfId="2"/>
-    <tableColumn id="10" name="Comment" dataDxfId="1"/>
+    <tableColumn id="1" name="Title/User Story" dataDxfId="9"/>
+    <tableColumn id="2" name="Description/Activity" dataDxfId="8"/>
+    <tableColumn id="3" name="Priority_x000a_(1 = high)" dataDxfId="7"/>
+    <tableColumn id="4" name="Estimated Time" dataDxfId="6"/>
+    <tableColumn id="5" name="Started/used" dataDxfId="5"/>
+    <tableColumn id="6" name="Completion used" dataDxfId="4"/>
+    <tableColumn id="7" name="Developer" dataDxfId="3"/>
+    <tableColumn id="8" name="Status" dataDxfId="2"/>
+    <tableColumn id="9" name="Week" dataDxfId="1"/>
+    <tableColumn id="10" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1188,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>27</v>
@@ -1214,47 +1226,47 @@
     </row>
     <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="19">
         <v>3</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="20">
         <v>2</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>27</v>
@@ -1275,40 +1287,40 @@
         <v>28</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="21">
         <v>3</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5" s="21">
         <v>0</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1322,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>27</v>
@@ -1357,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>27</v>
@@ -1378,38 +1390,38 @@
         <v>28</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="9">
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1423,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>27</v>
@@ -1449,16 +1461,16 @@
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="9">
         <v>3</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>27</v>
@@ -1477,7 +1489,7 @@
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1494,7 +1506,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1558,10 +1570,10 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="6">
         <v>0</v>
@@ -1570,12 +1582,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -1586,70 +1598,70 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="6">
         <v>0</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6">
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="6">
         <v>0</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1668,10 +1680,10 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -1696,10 +1708,10 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -1724,10 +1736,10 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
@@ -1736,38 +1748,38 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6">
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6">
         <v>3</v>
@@ -1778,22 +1790,23 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="6">
         <v>0</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>